<commit_message>
Added Queue item task
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karri\OneDrive\Documents\UiPath\AcmeCustomerSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karri\OneDrive\Documents\UiPath\ACMECustomerSecurityHashBOT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E8AFDF-F71E-4D9B-8E00-72203B395E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5981F3B-A8BF-454A-986B-A76CF5172EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -95,104 +95,109 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ACMECustomerSecurityHash</t>
+  </si>
+  <si>
+    <t>ACMEURL</t>
+  </si>
+  <si>
+    <t>SecurityHashURL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>ACMECreds</t>
+  </si>
+  <si>
+    <t>AttendedAssistantLow</t>
+  </si>
+  <si>
+    <t>AttendedAssistantTop</t>
+  </si>
+  <si>
+    <t>Copyright @shiva</t>
+  </si>
+  <si>
+    <t>ACMECredsAsset</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>ACMEWorkItemsURL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/home</t>
+  </si>
+  <si>
+    <t>ACMEHomepageURL</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ACMECustomerSecurityHash</t>
-  </si>
-  <si>
-    <t>CustomerSecurityHash</t>
-  </si>
-  <si>
-    <t>ACMEURL</t>
-  </si>
-  <si>
-    <t>SecurityHashURL</t>
-  </si>
-  <si>
-    <t>http://www.sha1-online.com/</t>
-  </si>
-  <si>
-    <t>ACMECreds</t>
-  </si>
-  <si>
-    <t>AttendedAssistantLow</t>
-  </si>
-  <si>
-    <t>AttendedAssistantTop</t>
-  </si>
-  <si>
-    <t>Copyright @shiva</t>
-  </si>
-  <si>
-    <t>ACMECredsAsset</t>
-  </si>
-  <si>
-    <t>https://acme-test.uipath.com/login</t>
-  </si>
-  <si>
-    <t>ACMEWorkItemsURL</t>
-  </si>
-  <si>
-    <t>https://acme-test.uipath.com/work-items</t>
+  </si>
+  <si>
+    <t>CustomerSecurityHashTest</t>
   </si>
 </sst>
 </file>
@@ -580,7 +585,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -627,10 +632,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -638,11 +643,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -651,7 +656,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -659,54 +664,61 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1698,9 +1710,10 @@
     <hyperlink ref="B6" r:id="rId1" xr:uid="{363C4FA5-590C-4472-B69D-5503A003C7F8}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{283D08AF-EDE6-4B7C-8DA7-2B23AFCBA73F}"/>
     <hyperlink ref="B12" r:id="rId3" xr:uid="{899BECF2-A226-47C1-8D1B-E0ED06464F7F}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{F94F4FE8-AF36-416F-B3E2-056CBE94BB77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1762,18 +1775,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1797,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1819,7 +1832,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1830,7 +1843,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1841,53 +1854,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2891,7 +2904,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added customer data fetch and SHA1 Launch
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karri\OneDrive\Documents\UiPath\ACMECustomerSecurityHashBOT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5981F3B-A8BF-454A-986B-A76CF5172EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315B93F5-C15B-4167-86B6-28DFCCC42058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>CustomerSecurityHashTest</t>
+  </si>
+  <si>
+    <t>ACMEWorkItemURL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -719,7 +725,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1711,9 +1724,10 @@
     <hyperlink ref="B7" r:id="rId2" xr:uid="{283D08AF-EDE6-4B7C-8DA7-2B23AFCBA73F}"/>
     <hyperlink ref="B12" r:id="rId3" xr:uid="{899BECF2-A226-47C1-8D1B-E0ED06464F7F}"/>
     <hyperlink ref="B13" r:id="rId4" xr:uid="{F94F4FE8-AF36-416F-B3E2-056CBE94BB77}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{58E57E93-7604-414E-AEB7-C5790E4B9811}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>